<commit_message>
Added ARC logo on PCB and generated output files
</commit_message>
<xml_diff>
--- a/Altium_Linda_SRAD_Avionics/Bill of Materials-Linda_SRAD_AvionicsV03.xlsx
+++ b/Altium_Linda_SRAD_Avionics/Bill of Materials-Linda_SRAD_AvionicsV03.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0857040a5fc6d13c/Desktop/Altium_Projects/Linda-Avionics-Hardware/Altium_Linda_SRAD_Avionics/Project Outputs for Linda_SRAD_Avionics/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0857040a5fc6d13c/Desktop/Altium_Projects/Linda-Avionics-Hardware/Altium_Linda_SRAD_Avionics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{79BD77D4-8251-4D09-938F-EC45512BDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AEEE8560-7B6F-4C69-8303-7DCBD607CFB1}"/>
+  <xr:revisionPtr revIDLastSave="277" documentId="8_{79BD77D4-8251-4D09-938F-EC45512BDE32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A64D6DDC-D634-49B4-BB7C-31D2538A572F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="197">
   <si>
     <t>Project Full Path</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>Rectifier Diodes</t>
-  </si>
-  <si>
-    <t>Resistors</t>
   </si>
   <si>
     <t>Terminal Blocks</t>
@@ -1576,14 +1573,20 @@
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1593,20 +1596,14 @@
       <alignment horizontal="left" vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2114,8 +2111,8 @@
   </sheetPr>
   <dimension ref="A1:O50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P49" sqref="P49"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2282,11 +2279,11 @@
       </c>
       <c r="D8" s="21">
         <f ca="1">TODAY()</f>
-        <v>44981</v>
+        <v>44982</v>
       </c>
       <c r="E8" s="22">
         <f ca="1">NOW()</f>
-        <v>44981.979155208333</v>
+        <v>44982.363258796293</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -2304,40 +2301,40 @@
         <v>41</v>
       </c>
       <c r="D9" s="36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E9" s="36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="36" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" s="36" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H9" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="I9" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="I9" s="36" t="s">
-        <v>116</v>
-      </c>
       <c r="J9" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K9" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="L9" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="L9" s="43" t="s">
+      <c r="M9" s="37" t="s">
         <v>135</v>
       </c>
-      <c r="M9" s="37" t="s">
+      <c r="N9" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="N9" s="37" t="s">
+      <c r="O9" s="37" t="s">
         <v>137</v>
-      </c>
-      <c r="O9" s="37" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2347,28 +2344,28 @@
         <v>1</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F10" s="30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H10" s="30">
         <v>1</v>
       </c>
       <c r="I10" s="74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K10" s="40">
         <v>5</v>
@@ -2393,28 +2390,28 @@
         <v>2</v>
       </c>
       <c r="C11" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="D11" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="32" t="s">
-        <v>149</v>
-      </c>
       <c r="E11" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G11" s="32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H11" s="32">
         <v>1</v>
       </c>
       <c r="I11" s="75" t="s">
+        <v>151</v>
+      </c>
+      <c r="J11" s="32" t="s">
         <v>152</v>
-      </c>
-      <c r="J11" s="32" t="s">
-        <v>153</v>
       </c>
       <c r="K11" s="41">
         <v>5</v>
@@ -2439,28 +2436,28 @@
         <v>3</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H12" s="30">
         <v>1</v>
       </c>
       <c r="I12" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K12" s="40">
         <v>50</v>
@@ -2485,28 +2482,28 @@
         <v>4</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H13" s="31">
         <v>1</v>
       </c>
-      <c r="I13" s="99" t="s">
-        <v>151</v>
+      <c r="I13" s="94" t="s">
+        <v>150</v>
       </c>
       <c r="J13" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K13" s="31">
         <v>10</v>
@@ -2531,28 +2528,28 @@
         <v>5</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D14" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="30" t="s">
         <v>161</v>
-      </c>
-      <c r="E14" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="G14" s="30" t="s">
-        <v>162</v>
       </c>
       <c r="H14" s="30">
         <v>1</v>
       </c>
       <c r="I14" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K14" s="40">
         <v>5</v>
@@ -2577,28 +2574,28 @@
         <v>6</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D15" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="E15" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G15" s="31" t="s">
         <v>165</v>
-      </c>
-      <c r="E15" s="31" t="s">
-        <v>167</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>166</v>
       </c>
       <c r="H15" s="31">
         <v>1</v>
       </c>
-      <c r="I15" s="99" t="s">
-        <v>151</v>
+      <c r="I15" s="94" t="s">
+        <v>150</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K15" s="31">
         <v>5</v>
@@ -2623,28 +2620,28 @@
         <v>7</v>
       </c>
       <c r="C16" s="28" t="s">
+        <v>168</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="E16" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>173</v>
-      </c>
-      <c r="E16" s="30" t="s">
+      <c r="F16" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="30" t="s">
         <v>170</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>146</v>
-      </c>
-      <c r="G16" s="30" t="s">
-        <v>171</v>
       </c>
       <c r="H16" s="30">
         <v>1</v>
       </c>
       <c r="I16" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K16" s="40">
         <v>6</v>
@@ -2669,26 +2666,26 @@
         <v>8</v>
       </c>
       <c r="C17" s="31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="31" t="s">
         <v>174</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>175</v>
       </c>
       <c r="E17" s="31"/>
       <c r="F17" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H17" s="31">
         <v>2</v>
       </c>
-      <c r="I17" s="99" t="s">
-        <v>151</v>
+      <c r="I17" s="94" t="s">
+        <v>150</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K17" s="31">
         <v>10</v>
@@ -2713,26 +2710,26 @@
         <v>9</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E18" s="30"/>
       <c r="F18" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H18" s="30">
         <v>2</v>
       </c>
       <c r="I18" s="74" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J18" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K18" s="40">
         <v>10</v>
@@ -2757,28 +2754,28 @@
         <v>10</v>
       </c>
       <c r="C19" s="31" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="31" t="s">
+        <v>181</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G19" s="31" t="s">
         <v>185</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="E19" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>186</v>
       </c>
       <c r="H19" s="31">
         <v>2</v>
       </c>
-      <c r="I19" s="99" t="s">
-        <v>151</v>
+      <c r="I19" s="94" t="s">
+        <v>150</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K19" s="31">
         <v>10</v>
@@ -2803,23 +2800,23 @@
         <v>11</v>
       </c>
       <c r="C20" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="28" t="s">
         <v>187</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>188</v>
       </c>
       <c r="E20" s="30"/>
       <c r="F20" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H20" s="30">
         <v>5</v>
       </c>
       <c r="I20" s="74" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J20" s="30"/>
       <c r="K20" s="40">
@@ -2845,28 +2842,28 @@
         <v>12</v>
       </c>
       <c r="C21" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="32" t="s">
-        <v>146</v>
-      </c>
       <c r="E21" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F21" s="32" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G21" s="32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H21" s="32">
         <v>4</v>
       </c>
       <c r="I21" s="75" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J21" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K21" s="32">
         <v>0</v>
@@ -2894,25 +2891,25 @@
         <v>42</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" s="30" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H22" s="30">
         <v>2</v>
       </c>
       <c r="I22" s="74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J22" s="30" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K22" s="40">
         <v>10</v>
@@ -2940,25 +2937,25 @@
         <v>43</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G23" s="32" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H23" s="32">
         <v>4</v>
       </c>
       <c r="I23" s="75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J23" s="32" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K23" s="41">
         <v>20</v>
@@ -2986,25 +2983,25 @@
         <v>43</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H24" s="30">
         <v>1</v>
       </c>
       <c r="I24" s="74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J24" s="30" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K24" s="40">
         <v>5</v>
@@ -3032,25 +3029,25 @@
         <v>43</v>
       </c>
       <c r="D25" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E25" s="32" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F25" s="32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G25" s="32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H25" s="32">
         <v>1</v>
       </c>
       <c r="I25" s="75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J25" s="32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K25" s="41">
         <v>5</v>
@@ -3078,25 +3075,25 @@
         <v>44</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H26" s="30">
         <v>3</v>
       </c>
       <c r="I26" s="74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K26" s="40">
         <v>15</v>
@@ -3124,25 +3121,25 @@
         <v>44</v>
       </c>
       <c r="D27" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E27" s="32" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G27" s="32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H27" s="32">
         <v>1</v>
       </c>
       <c r="I27" s="75" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J27" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K27" s="41">
         <v>5</v>
@@ -3170,25 +3167,25 @@
         <v>44</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F28" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H28" s="30">
         <v>2</v>
       </c>
       <c r="I28" s="74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J28" s="30" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="K28" s="40">
         <v>10</v>
@@ -3216,25 +3213,25 @@
         <v>44</v>
       </c>
       <c r="D29" s="32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H29" s="32">
         <v>1</v>
       </c>
       <c r="I29" s="75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J29" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K29" s="41">
         <v>5</v>
@@ -3262,25 +3259,25 @@
         <v>44</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F30" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G30" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H30" s="30">
         <v>1</v>
       </c>
       <c r="I30" s="74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J30" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K30" s="40">
         <v>5</v>
@@ -3308,25 +3305,25 @@
         <v>45</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F31" s="32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G31" s="32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H31" s="32">
         <v>1</v>
       </c>
       <c r="I31" s="75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J31" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K31" s="41">
         <v>5</v>
@@ -3354,25 +3351,25 @@
         <v>46</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G32" s="30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H32" s="30">
         <v>1</v>
       </c>
       <c r="I32" s="74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J32" s="30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K32" s="40">
         <v>5</v>
@@ -3400,25 +3397,25 @@
         <v>46</v>
       </c>
       <c r="D33" s="32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F33" s="32" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G33" s="32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H33" s="32">
         <v>3</v>
       </c>
       <c r="I33" s="75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J33" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K33" s="41">
         <v>15</v>
@@ -3446,25 +3443,25 @@
         <v>47</v>
       </c>
       <c r="D34" s="28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F34" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G34" s="30" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H34" s="30">
         <v>1</v>
       </c>
       <c r="I34" s="74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J34" s="30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K34" s="40">
         <v>5</v>
@@ -3492,25 +3489,25 @@
         <v>48</v>
       </c>
       <c r="D35" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F35" s="32" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G35" s="32" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H35" s="32">
         <v>2</v>
       </c>
       <c r="I35" s="75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J35" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K35" s="41">
         <v>10</v>
@@ -3535,28 +3532,28 @@
         <v>27</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G36" s="30" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H36" s="30">
         <v>2</v>
       </c>
       <c r="I36" s="74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J36" s="30" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K36" s="40">
         <v>10</v>
@@ -3581,28 +3578,28 @@
         <v>28</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F37" s="32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G37" s="32" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H37" s="32">
         <v>2</v>
       </c>
       <c r="I37" s="75" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J37" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K37" s="41">
         <v>10</v>
@@ -3627,28 +3624,28 @@
         <v>29</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F38" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G38" s="30" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H38" s="30">
         <v>1</v>
       </c>
       <c r="I38" s="74" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J38" s="30" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K38" s="40">
         <v>5</v>
@@ -3692,10 +3689,10 @@
     </row>
     <row r="40" spans="1:15" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="55"/>
-      <c r="B40" s="97" t="s">
+      <c r="B40" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="98"/>
+      <c r="C40" s="100"/>
       <c r="D40" s="5"/>
       <c r="E40" s="7"/>
       <c r="F40" s="49" t="s">
@@ -3723,11 +3720,11 @@
       <c r="J41" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="L41" s="94">
+      <c r="L41" s="101">
         <f>N39</f>
         <v>597.1</v>
       </c>
-      <c r="M41" s="95"/>
+      <c r="M41" s="102"/>
       <c r="N41" s="89" t="s">
         <v>40</v>
       </c>
@@ -3747,11 +3744,11 @@
         <v>28</v>
       </c>
       <c r="K42" s="6"/>
-      <c r="L42" s="96">
+      <c r="L42" s="103">
         <f>L41/H41</f>
         <v>119.42</v>
       </c>
-      <c r="M42" s="96"/>
+      <c r="M42" s="103"/>
       <c r="N42" s="90" t="s">
         <v>40</v>
       </c>
@@ -3778,24 +3775,24 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="J45" s="100" t="s">
-        <v>193</v>
-      </c>
-      <c r="K45" s="100"/>
+      <c r="J45" s="95" t="s">
+        <v>192</v>
+      </c>
+      <c r="K45" s="95"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="J46" s="100" t="s">
-        <v>194</v>
-      </c>
-      <c r="K46" s="101">
+      <c r="J46" s="95" t="s">
+        <v>193</v>
+      </c>
+      <c r="K46" s="96">
         <f>L42-M10-M12-M13-M14-M15-M16-M19-M18-M17</f>
         <v>67.670000000000016</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.2">
@@ -3803,15 +3800,15 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="L47" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="50" spans="10:14" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="J50" s="97" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="50" spans="10:14" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="J50" s="102" t="s">
-        <v>197</v>
-      </c>
-      <c r="K50" s="102"/>
-      <c r="N50" s="103">
+      <c r="K50" s="97"/>
+      <c r="N50" s="98">
         <f>SUM(N10,N20,N22:N30,N32,N33,N34,N35,N36)</f>
         <v>105.54</v>
       </c>
@@ -3866,7 +3863,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="91" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3898,7 +3895,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="93" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3914,7 +3911,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="93" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3938,7 +3935,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="92" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3946,7 +3943,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="93" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3954,7 +3951,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3962,7 +3959,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="93" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3970,7 +3967,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>